<commit_message>
Update BOM; Generate Gerbers
</commit_message>
<xml_diff>
--- a/ValveDriver_BOM.xlsx
+++ b/ValveDriver_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10312"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ofer/src/HMS_8_Valve_Driver/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ofer/Dropbox (HMS)/RIC/Projects/8 Ch Valve Driver/HMS-8-Valve-Driver/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE54E78D-91C1-704C-B876-5D4D2D2B9667}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A0DD023-BAB4-514E-90F1-F8992BC6577C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17840" yWindow="9540" windowWidth="23120" windowHeight="14000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ValveDriver_BOM.csv" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
-  <si>
-    <t>Part</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Value</t>
   </si>
@@ -45,87 +42,12 @@
     <t>J1</t>
   </si>
   <si>
-    <t>CONN_10",1X10"</t>
-  </si>
-  <si>
-    <t>J3</t>
-  </si>
-  <si>
-    <t>CONN_083.5MM-8</t>
-  </si>
-  <si>
     <t>J4</t>
   </si>
   <si>
     <t>POWER_JACK</t>
   </si>
   <si>
-    <t>J5</t>
-  </si>
-  <si>
-    <t>Valve 8</t>
-  </si>
-  <si>
-    <t>CONN_02</t>
-  </si>
-  <si>
-    <t>J6</t>
-  </si>
-  <si>
-    <t>Valve 7</t>
-  </si>
-  <si>
-    <t>J7</t>
-  </si>
-  <si>
-    <t>Valve 6</t>
-  </si>
-  <si>
-    <t>J8</t>
-  </si>
-  <si>
-    <t>Valve 5</t>
-  </si>
-  <si>
-    <t>J9</t>
-  </si>
-  <si>
-    <t>Valve 4</t>
-  </si>
-  <si>
-    <t>J10</t>
-  </si>
-  <si>
-    <t>Valve 3</t>
-  </si>
-  <si>
-    <t>J11</t>
-  </si>
-  <si>
-    <t>Valve 2</t>
-  </si>
-  <si>
-    <t>J12</t>
-  </si>
-  <si>
-    <t>Valve 1</t>
-  </si>
-  <si>
-    <t>J13</t>
-  </si>
-  <si>
-    <t>J14</t>
-  </si>
-  <si>
-    <t>CONN_04</t>
-  </si>
-  <si>
-    <t>U$1</t>
-  </si>
-  <si>
-    <t>TEENSY_3.1-3.2_DIL</t>
-  </si>
-  <si>
     <t>Digikey part</t>
   </si>
   <si>
@@ -138,22 +60,64 @@
     <t xml:space="preserve">497-2356-5-ND </t>
   </si>
   <si>
-    <t>Buy from PJRC: https://www.pjrc.com/store/teensy32_pins.html</t>
-  </si>
-  <si>
-    <t>TEENSY32_PINS</t>
-  </si>
-  <si>
-    <t>14-pin sockets (2x)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> S7012-ND</t>
-  </si>
-  <si>
-    <t>WM7864-ND</t>
-  </si>
-  <si>
     <t>Can also use ULQ2803A (497-2362-5-ND)</t>
+  </si>
+  <si>
+    <t>0.1" Header 1X10"</t>
+  </si>
+  <si>
+    <t>J5–12</t>
+  </si>
+  <si>
+    <t>J15–18</t>
+  </si>
+  <si>
+    <t>BNC connector</t>
+  </si>
+  <si>
+    <t>WM5514-ND</t>
+  </si>
+  <si>
+    <t>S1–4</t>
+  </si>
+  <si>
+    <t>Ref</t>
+  </si>
+  <si>
+    <t>1528-367-ND</t>
+  </si>
+  <si>
+    <t>(Bag of 20x)</t>
+  </si>
+  <si>
+    <t>6mm tactile switch</t>
+  </si>
+  <si>
+    <t>A98333-ND</t>
+  </si>
+  <si>
+    <t>Screw Terminal</t>
+  </si>
+  <si>
+    <t>S7035-ND</t>
+  </si>
+  <si>
+    <t>Socket</t>
+  </si>
+  <si>
+    <t>Valve connector (option A)</t>
+  </si>
+  <si>
+    <t>Valve connector (option B)</t>
+  </si>
+  <si>
+    <t>CP-202A-ND</t>
+  </si>
+  <si>
+    <t>S7043-ND</t>
+  </si>
+  <si>
+    <t>NOTE: All components besides the driver chip (IC1) are commodity parts and can be swapped with suitable alternatives</t>
   </si>
 </sst>
 </file>
@@ -172,19 +136,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="12"/>
       <color theme="10"/>
@@ -196,6 +147,21 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -220,21 +186,21 @@
   </borders>
   <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -582,16 +548,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="10.83203125" style="1"/>
-    <col min="3" max="3" width="17.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="17.5" style="1" customWidth="1"/>
     <col min="5" max="5" width="19.6640625" style="4" customWidth="1"/>
     <col min="6" max="6" width="27" style="1" customWidth="1"/>
@@ -600,204 +566,131 @@
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="E2" s="4">
         <v>2.8</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0.68</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.7</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>26</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.33</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>27</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>13</v>
+      <c r="D7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="4">
+        <v>2.5</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>13</v>
+      <c r="F8" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E16" s="4">
-        <v>22.8</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C17" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E17" s="4">
-        <v>0.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>